<commit_message>
app and flex sensor commit
</commit_message>
<xml_diff>
--- a/mesures_fleche.xlsx
+++ b/mesures_fleche.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Desktop\Projet_Capteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>Def (cm)</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <t>Angle (°)</t>
+  </si>
+  <si>
+    <t>Flex sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L sensor = </t>
   </si>
 </sst>
 </file>
@@ -3469,6 +3475,1039 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Sensibilité du </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" i="1"/>
+              <a:t>Flex sensor </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" i="0"/>
+              <a:t>commercial</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.11128762029746292"/>
+                  <c:y val="7.3657407407407408E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$U$28:$U$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.885527054658738</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.090816348852169</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.037511025421814</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.676815681838217</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29.981639368849329</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$U$11:$U$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.7972508591065368E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12409240924092414</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.14662379421221872</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.19085365853658531</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.23515850144092229</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7AA9-4517-8FF2-F9626D323B8A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="773372720"/>
+        <c:axId val="773379376"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="773372720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Angle de courbure (deg)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="773379376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="773379376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="el-GR"/>
+                  <a:t>Δ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>R/R</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="773372720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Sensibilité du </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" i="1"/>
+              <a:t>Flex sensor </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" i="0"/>
+              <a:t>commercial</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.11128762029746292"/>
+                  <c:y val="7.3657407407407408E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$U$28:$U$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.885527054658738</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.090816348852169</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.037511025421814</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.676815681838217</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29.981639368849329</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$V$11:$V$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.937984496124031E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.137254901960787E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-4.7808764940239015E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-6.048387096774193E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D95D-489A-AB42-A118D390C05F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="773372720"/>
+        <c:axId val="773379376"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="773372720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Angle de courbure (deg)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="773379376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="773379376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="el-GR"/>
+                  <a:t>Δ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>R/R</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="773372720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3589,6 +4628,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4622,6 +5741,1038 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5226,6 +7377,68 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>110490</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>110490</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Graphique 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5497,10 +7710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S37"/>
+  <dimension ref="A1:V38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="G22" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5508,7 +7721,7 @@
     <col min="6" max="7" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>23</v>
       </c>
@@ -5560,8 +7773,11 @@
       <c r="S1" t="s">
         <v>39</v>
       </c>
+      <c r="U1" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -5619,8 +7835,14 @@
       <c r="S2">
         <v>20.3</v>
       </c>
+      <c r="U2">
+        <v>26.54</v>
+      </c>
+      <c r="V2">
+        <v>26.3</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>1</v>
       </c>
@@ -5675,8 +7897,14 @@
       <c r="S3">
         <v>20.8</v>
       </c>
+      <c r="U3">
+        <v>29.1</v>
+      </c>
+      <c r="V3">
+        <v>25.8</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>1.5</v>
       </c>
@@ -5731,8 +7959,14 @@
       <c r="S4">
         <v>21.1</v>
       </c>
+      <c r="U4">
+        <v>30.3</v>
+      </c>
+      <c r="V4">
+        <v>25.5</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>2</v>
       </c>
@@ -5787,8 +8021,14 @@
       <c r="S5">
         <v>21.6</v>
       </c>
+      <c r="U5">
+        <v>31.1</v>
+      </c>
+      <c r="V5">
+        <v>25.1</v>
+      </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>2.5</v>
       </c>
@@ -5831,8 +8071,14 @@
       <c r="S6">
         <v>22</v>
       </c>
+      <c r="U6">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="V6">
+        <v>24.8</v>
+      </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>3</v>
       </c>
@@ -5854,8 +8100,11 @@
       <c r="Q7">
         <v>16.7</v>
       </c>
+      <c r="U7">
+        <v>34.700000000000003</v>
+      </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>1</v>
       </c>
@@ -5863,7 +8112,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>0</v>
       </c>
@@ -5935,8 +8184,16 @@
         <f>(S2-$S$2)/$S$2</f>
         <v>0</v>
       </c>
+      <c r="U11">
+        <f>(U2-$U$2)/U2</f>
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <f>(V2-$V$2)/V2</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>1</v>
       </c>
@@ -5973,7 +8230,7 @@
         <v>2.5531914893617082E-2</v>
       </c>
       <c r="K12">
-        <f t="shared" ref="K12:K15" si="8">(K3-$K$2)/$K$2</f>
+        <f t="shared" ref="K12:K14" si="8">(K3-$K$2)/$K$2</f>
         <v>-5.128205128205128E-2</v>
       </c>
       <c r="L12">
@@ -6005,11 +8262,19 @@
         <v>5.235602094240837E-2</v>
       </c>
       <c r="S12">
-        <f t="shared" ref="S12:S16" si="16">(S3-$S$2)/$S$2</f>
+        <f t="shared" ref="S12:S15" si="16">(S3-$S$2)/$S$2</f>
         <v>2.463054187192118E-2</v>
       </c>
+      <c r="U12">
+        <f t="shared" ref="U12:U16" si="17">(U3-$U$2)/U3</f>
+        <v>8.7972508591065368E-2</v>
+      </c>
+      <c r="V12">
+        <f t="shared" ref="V12:V15" si="18">(V3-$V$2)/V3</f>
+        <v>-1.937984496124031E-2</v>
+      </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>1.5</v>
       </c>
@@ -6081,8 +8346,16 @@
         <f t="shared" si="16"/>
         <v>3.9408866995073927E-2</v>
       </c>
+      <c r="U13">
+        <f t="shared" si="17"/>
+        <v>0.12409240924092414</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="18"/>
+        <v>-3.137254901960787E-2</v>
+      </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>2</v>
       </c>
@@ -6154,8 +8427,16 @@
         <f t="shared" si="16"/>
         <v>6.4039408866995107E-2</v>
       </c>
+      <c r="U14">
+        <f t="shared" si="17"/>
+        <v>0.14662379421221872</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="18"/>
+        <v>-4.7808764940239015E-2</v>
+      </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>2.5</v>
       </c>
@@ -6223,8 +8504,16 @@
         <f t="shared" si="16"/>
         <v>8.3743842364531987E-2</v>
       </c>
+      <c r="U15">
+        <f t="shared" si="17"/>
+        <v>0.19085365853658531</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="18"/>
+        <v>-6.048387096774193E-2</v>
+      </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>3</v>
       </c>
@@ -6264,8 +8553,12 @@
         <f t="shared" si="14"/>
         <v>-0.12565445026178021</v>
       </c>
+      <c r="U16">
+        <f t="shared" si="17"/>
+        <v>0.23515850144092229</v>
+      </c>
     </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C18" s="3" t="s">
         <v>3</v>
       </c>
@@ -6318,20 +8611,20 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19" s="2">
-        <f t="shared" ref="C19:E24" si="17">C11*100</f>
+        <f t="shared" ref="C19:E24" si="19">C11*100</f>
         <v>0</v>
       </c>
       <c r="D19" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="E19">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="F19">
@@ -6343,27 +8636,27 @@
         <v>0</v>
       </c>
       <c r="H19">
-        <f t="shared" ref="H19:S19" si="18">H11*100</f>
+        <f t="shared" ref="H19:S19" si="20">H11*100</f>
         <v>0</v>
       </c>
       <c r="I19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="J19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="K19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="L19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="M19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N19">
@@ -6371,332 +8664,332 @@
         <v>0</v>
       </c>
       <c r="O19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="P19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="R19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="S19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-4.9504950495049505</v>
       </c>
       <c r="D20" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-3.8834951456310711</v>
       </c>
       <c r="E20">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-2.8985507246376812</v>
       </c>
       <c r="F20">
-        <f t="shared" ref="F20:F22" si="19">100*F12</f>
+        <f t="shared" ref="F20:F22" si="21">100*F12</f>
         <v>5.0335570469798654</v>
       </c>
       <c r="G20">
-        <f t="shared" ref="G20:S20" si="20">G12*100</f>
+        <f t="shared" ref="G20:S20" si="22">G12*100</f>
         <v>2.760736196319014</v>
       </c>
       <c r="H20">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.7191977077363938</v>
       </c>
       <c r="I20">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>-3.6144578313253093</v>
       </c>
       <c r="J20">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>2.553191489361708</v>
       </c>
       <c r="K20">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>-5.1282051282051277</v>
       </c>
       <c r="L20">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>3.4782608695652204</v>
       </c>
       <c r="M20">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>-3.5087719298245648</v>
       </c>
       <c r="N20">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>4.8964218455743902</v>
       </c>
       <c r="O20">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>-2.7548209366391188</v>
       </c>
       <c r="P20">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>3.4090909090908972</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>-3.6649214659686007</v>
       </c>
       <c r="R20">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>5.2356020942408366</v>
       </c>
       <c r="S20">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>2.4630541871921179</v>
       </c>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>1.5</v>
       </c>
       <c r="C21" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-8.9108910891089099</v>
       </c>
       <c r="D21" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-5.8252427184466153</v>
       </c>
       <c r="E21">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-4.3478260869565215</v>
       </c>
       <c r="F21">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>6.3758389261744917</v>
       </c>
       <c r="G21">
-        <f t="shared" ref="G21:S21" si="21">G13*100</f>
+        <f t="shared" ref="G21:S21" si="23">G13*100</f>
         <v>5.521472392638028</v>
       </c>
       <c r="H21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>2.8653295128939829</v>
       </c>
       <c r="I21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>-5.120481927710852</v>
       </c>
       <c r="J21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>4.2553191489361701</v>
       </c>
       <c r="K21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>-6.6666666666666705</v>
       </c>
       <c r="L21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>6.9565217391304408</v>
       </c>
       <c r="M21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>-8.7719298245614024</v>
       </c>
       <c r="N21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>6.5913370998116756</v>
       </c>
       <c r="O21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>-3.9944903581267099</v>
       </c>
       <c r="P21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>6.2499999999999876</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>-5.7591623036649287</v>
       </c>
       <c r="R21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>7.8534031413612562</v>
       </c>
       <c r="S21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.9408866995073928</v>
       </c>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>2</v>
       </c>
       <c r="C22" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-10.099009900990103</v>
       </c>
       <c r="D22" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-9.2233009708737956</v>
       </c>
       <c r="E22">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-5.5072463768115902</v>
       </c>
       <c r="F22">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>8.0536912751677914</v>
       </c>
       <c r="G22">
-        <f t="shared" ref="G22:S22" si="22">G14*100</f>
+        <f t="shared" ref="G22:S22" si="24">G14*100</f>
         <v>7.6687116564417179</v>
       </c>
       <c r="H22">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>5.1575931232091818</v>
       </c>
       <c r="I22">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>-9.3373493975903656</v>
       </c>
       <c r="J22">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>5.9574468085106327</v>
       </c>
       <c r="K22">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>-8.7179487179487154</v>
       </c>
       <c r="L22">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>10.434782608695645</v>
       </c>
       <c r="M22">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>-10.526315789473694</v>
       </c>
       <c r="N22">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>10.169491525423725</v>
       </c>
       <c r="O22">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>-5.3719008264462698</v>
       </c>
       <c r="P22">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>11.363636363636363</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>-7.3298429319371836</v>
       </c>
       <c r="R22">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>9.4240837696334925</v>
       </c>
       <c r="S22">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>6.4039408866995107</v>
       </c>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>2.5</v>
       </c>
       <c r="C23" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-13.861386138613863</v>
       </c>
       <c r="D23" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-11.165048543689323</v>
       </c>
       <c r="E23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-6.956521739130431</v>
       </c>
       <c r="G23">
-        <f t="shared" ref="G23:K23" si="23">G15*100</f>
+        <f t="shared" ref="G23:J23" si="25">G15*100</f>
         <v>9.8159509202453847</v>
       </c>
       <c r="H23">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>6.8767908309455548</v>
       </c>
       <c r="I23">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>-10.240963855421692</v>
       </c>
       <c r="J23">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>7.6595744680851094</v>
       </c>
       <c r="N23">
-        <f t="shared" ref="M23:S24" si="24">N15*100</f>
+        <f t="shared" ref="N23:S24" si="26">N15*100</f>
         <v>12.806026365348394</v>
       </c>
       <c r="O23">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>-7.1625344352616933</v>
       </c>
       <c r="P23">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>13.636363636363628</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>-8.9005235602094377</v>
       </c>
       <c r="R23">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>12.04188481675391</v>
       </c>
       <c r="S23">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>8.3743842364531993</v>
       </c>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>3</v>
       </c>
       <c r="C24" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-19.009900990099013</v>
       </c>
       <c r="D24" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-13.592233009708741</v>
       </c>
       <c r="E24">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-7.8260869565217366</v>
       </c>
       <c r="I24">
-        <f t="shared" ref="I24:K24" si="25">I16*100</f>
+        <f t="shared" ref="I24" si="27">I16*100</f>
         <v>-12.34939759036145</v>
       </c>
       <c r="N24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>15.442561205273062</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>-12.56544502617802</v>
       </c>
     </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>0</v>
       </c>
@@ -6724,8 +9017,14 @@
       <c r="M27" t="s">
         <v>45</v>
       </c>
+      <c r="T27" t="s">
+        <v>44</v>
+      </c>
+      <c r="U27" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>0</v>
       </c>
@@ -6734,15 +9033,15 @@
         <v>0</v>
       </c>
       <c r="D28">
-        <f>AVERAGE(E19,I19)</f>
+        <f t="shared" ref="D28:D33" si="28">AVERAGE(E19,I19)</f>
         <v>0</v>
       </c>
       <c r="F28">
-        <f>AVERAGE(J19,L19)</f>
+        <f t="shared" ref="F28:G31" si="29">AVERAGE(J19,L19)</f>
         <v>0</v>
       </c>
       <c r="G28">
-        <f>AVERAGE(K19,M19)</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="I28">
@@ -6761,8 +9060,16 @@
         <f>L28/(PI()/180)</f>
         <v>0</v>
       </c>
+      <c r="T28" s="2">
+        <f>ATAN(B28/$C$38)</f>
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <f>T28/(PI()/180)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>1</v>
       </c>
@@ -6771,35 +9078,43 @@
         <v>3.1711636503450911</v>
       </c>
       <c r="D29">
-        <f>AVERAGE(E20,I20)</f>
+        <f t="shared" si="28"/>
         <v>-3.2565042779814952</v>
       </c>
       <c r="F29">
-        <f>AVERAGE(J20,L20)</f>
+        <f t="shared" si="29"/>
         <v>3.0157261794634644</v>
       </c>
       <c r="G29">
-        <f>AVERAGE(K20,M20)</f>
+        <f t="shared" si="29"/>
         <v>-4.3184885290148465</v>
       </c>
       <c r="I29">
-        <f t="shared" ref="I29:I33" si="26">AVERAGE(S20,R20,P20,N20)</f>
+        <f t="shared" ref="I29:I33" si="30">AVERAGE(S20,R20,P20,N20)</f>
         <v>4.0010422590245609</v>
       </c>
       <c r="J29" s="2">
-        <f t="shared" ref="J29:J33" si="27">AVERAGE(Q20,O20,D20)</f>
+        <f t="shared" ref="J29:J33" si="31">AVERAGE(Q20,O20,D20)</f>
         <v>-3.4344125160795969</v>
       </c>
       <c r="L29">
-        <f>ATAN(B29/$C$37)</f>
+        <f t="shared" ref="L28:L33" si="32">ATAN(B29/$C$37)</f>
         <v>0.30288486837497142</v>
       </c>
       <c r="M29" s="2">
-        <f t="shared" ref="M29:M33" si="28">L29/(PI()/180)</f>
+        <f t="shared" ref="M29:M33" si="33">L29/(PI()/180)</f>
         <v>17.354024636261322</v>
       </c>
+      <c r="T29" s="2">
+        <f t="shared" ref="T29:T33" si="34">ATAN(B29/$C$38)</f>
+        <v>0.18998828791871572</v>
+      </c>
+      <c r="U29">
+        <f t="shared" ref="U29:U33" si="35">T29/(PI()/180)</f>
+        <v>10.885527054658738</v>
+      </c>
     </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>1.5</v>
       </c>
@@ -6808,35 +9123,43 @@
         <v>4.9208802772355007</v>
       </c>
       <c r="D30">
-        <f>AVERAGE(E21,I21)</f>
+        <f t="shared" si="28"/>
         <v>-4.7341540073336867</v>
       </c>
       <c r="F30">
-        <f>AVERAGE(J21,L21)</f>
+        <f t="shared" si="29"/>
         <v>5.6059204440333055</v>
       </c>
       <c r="G30">
-        <f>AVERAGE(K21,M21)</f>
+        <f t="shared" si="29"/>
         <v>-7.719298245614036</v>
       </c>
       <c r="I30">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>6.1589067351700777</v>
       </c>
       <c r="J30" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-5.1929651267460848</v>
       </c>
       <c r="L30">
-        <f>ATAN(B30/$C$37)</f>
+        <f t="shared" si="32"/>
         <v>0.43833655985795783</v>
       </c>
       <c r="M30" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>25.114834886144564</v>
       </c>
+      <c r="T30" s="2">
+        <f t="shared" si="34"/>
+        <v>0.28083772462120282</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="35"/>
+        <v>16.090816348852169</v>
+      </c>
     </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>2</v>
       </c>
@@ -6845,35 +9168,43 @@
         <v>6.9599986849395634</v>
       </c>
       <c r="D31">
-        <f>AVERAGE(E22,I22)</f>
+        <f t="shared" si="28"/>
         <v>-7.4222978872009779</v>
       </c>
       <c r="F31">
-        <f>AVERAGE(J22,L22)</f>
+        <f t="shared" si="29"/>
         <v>8.1961147086031385</v>
       </c>
       <c r="G31">
-        <f>AVERAGE(K22,M22)</f>
+        <f t="shared" si="29"/>
         <v>-9.6221322537112037</v>
       </c>
       <c r="I31">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>9.3402881363482724</v>
       </c>
       <c r="J31" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-7.3083482430857503</v>
       </c>
       <c r="L31">
-        <f>ATAN(B31/$C$37)</f>
+        <f t="shared" si="32"/>
         <v>0.55859931534356244</v>
       </c>
       <c r="M31" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>32.005383208083494</v>
       </c>
+      <c r="T31" s="2">
+        <f t="shared" si="34"/>
+        <v>0.36717383381821916</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="35"/>
+        <v>21.037511025421814</v>
+      </c>
     </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>2.5</v>
       </c>
@@ -6882,57 +9213,81 @@
         <v>8.3463708755954702</v>
       </c>
       <c r="D32">
-        <f>AVERAGE(E23,I23)</f>
+        <f t="shared" si="28"/>
         <v>-8.5987427972760617</v>
       </c>
       <c r="I32">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>11.714664763729782</v>
       </c>
       <c r="J32" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-9.0760355130534851</v>
       </c>
       <c r="L32">
-        <f>ATAN(B32/$C$37)</f>
+        <f t="shared" si="32"/>
         <v>0.66320299270609329</v>
       </c>
       <c r="M32" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>37.998732442504661</v>
       </c>
+      <c r="T32" s="2">
+        <f t="shared" si="34"/>
+        <v>0.44814497507578965</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="35"/>
+        <v>25.676815681838217</v>
+      </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>3</v>
       </c>
       <c r="D33">
-        <f>AVERAGE(E24,I24)</f>
+        <f t="shared" si="28"/>
         <v>-10.087742273441593</v>
       </c>
       <c r="I33">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>15.442561205273062</v>
       </c>
       <c r="J33" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-13.07883901794338</v>
       </c>
       <c r="L33">
-        <f>ATAN(B33/$C$37)</f>
+        <f t="shared" si="32"/>
         <v>0.75315128096219441</v>
       </c>
       <c r="M33" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>43.152389734005403</v>
       </c>
+      <c r="T33" s="2">
+        <f t="shared" si="34"/>
+        <v>0.52327832213197545</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="35"/>
+        <v>29.981639368849329</v>
+      </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>43</v>
       </c>
       <c r="C37">
         <v>3.2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38">
+        <v>5.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>